<commit_message>
Solved error that prevented the deletion of the savedatas
</commit_message>
<xml_diff>
--- a/Estadisticas Personages.xlsx
+++ b/Estadisticas Personages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Desktop\DTA\D-tector-Unity\D-Tector-v2-master\D-Tector-v2-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA349CDF-F405-4259-8F2D-AAFF3EA81E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497652E8-5216-4F71-B6DD-C04C5016E9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,13 @@
     <sheet name="ZO" sheetId="5" r:id="rId5"/>
     <sheet name="TM" sheetId="6" r:id="rId6"/>
     <sheet name="KH" sheetId="7" r:id="rId7"/>
+    <sheet name="SPIRIT HUMAN TIERRA" sheetId="12" r:id="rId8"/>
+    <sheet name="SPIRIT ANIMAL TIERRA " sheetId="13" r:id="rId9"/>
+    <sheet name="Hoja2" sheetId="14" r:id="rId10"/>
+    <sheet name="zulogmon bta trueno" sheetId="8" r:id="rId11"/>
+    <sheet name="bestia tigre bta2" sheetId="9" r:id="rId12"/>
+    <sheet name="bta3 dragon rojo" sheetId="10" r:id="rId13"/>
+    <sheet name="BTA4 TORTUGA" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="218">
   <si>
     <t>Koji</t>
   </si>
@@ -1003,13 +1010,127 @@
   </si>
   <si>
     <t xml:space="preserve"> es posible en el 71 que lleguen al máximo de capacidades</t>
+  </si>
+  <si>
+    <t>LV1</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>cr</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>lv</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>Boss name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Crush</t>
+  </si>
+  <si>
+    <t>Ability</t>
+  </si>
+  <si>
+    <t>Malomyotismon</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Megidramon</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Duskmon</t>
+  </si>
+  <si>
+    <t>Velgrmon</t>
+  </si>
+  <si>
+    <t>Grumblemon</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Gigasmon</t>
+  </si>
+  <si>
+    <t>Arbormon</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Petaldramon</t>
+  </si>
+  <si>
+    <t>Lanamon</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Calmaramon</t>
+  </si>
+  <si>
+    <t>Mercurymon</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Sephirothmon</t>
+  </si>
+  <si>
+    <t>Kerpymon (Fake Cherubimon - white)</t>
+  </si>
+  <si>
+    <t>Kerpymon (Real Cherubimon - black)</t>
+  </si>
+  <si>
+    <t>Ebonwumon</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Zhuqiaomon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1046,8 +1167,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1060,8 +1194,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3E4A64"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1069,11 +1215,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE0E0E0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE0E0E0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE0E0E0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1083,6 +1244,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1377,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="53" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -7297,6 +7467,562 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD7583-C875-4963-8091-856C9C26F0CF}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="7">
+        <v>220</v>
+      </c>
+      <c r="D2" s="7">
+        <v>200</v>
+      </c>
+      <c r="E2" s="7">
+        <v>100</v>
+      </c>
+      <c r="F2" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="8">
+        <v>230</v>
+      </c>
+      <c r="D3" s="8">
+        <v>180</v>
+      </c>
+      <c r="E3" s="8">
+        <v>200</v>
+      </c>
+      <c r="F3" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="7">
+        <v>160</v>
+      </c>
+      <c r="D4" s="7">
+        <v>120</v>
+      </c>
+      <c r="E4" s="7">
+        <v>120</v>
+      </c>
+      <c r="F4" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="8">
+        <v>220</v>
+      </c>
+      <c r="D5" s="8">
+        <v>140</v>
+      </c>
+      <c r="E5" s="8">
+        <v>180</v>
+      </c>
+      <c r="F5" s="8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="7">
+        <v>180</v>
+      </c>
+      <c r="D6" s="7">
+        <v>105</v>
+      </c>
+      <c r="E6" s="7">
+        <v>130</v>
+      </c>
+      <c r="F6" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="8">
+        <v>230</v>
+      </c>
+      <c r="D7" s="8">
+        <v>150</v>
+      </c>
+      <c r="E7" s="8">
+        <v>170</v>
+      </c>
+      <c r="F7" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="7">
+        <v>130</v>
+      </c>
+      <c r="D8" s="7">
+        <v>100</v>
+      </c>
+      <c r="E8" s="7">
+        <v>130</v>
+      </c>
+      <c r="F8" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="8">
+        <v>190</v>
+      </c>
+      <c r="D9" s="8">
+        <v>180</v>
+      </c>
+      <c r="E9" s="8">
+        <v>140</v>
+      </c>
+      <c r="F9" s="8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="7">
+        <v>100</v>
+      </c>
+      <c r="D10" s="7">
+        <v>120</v>
+      </c>
+      <c r="E10" s="7">
+        <v>120</v>
+      </c>
+      <c r="F10" s="7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="8">
+        <v>170</v>
+      </c>
+      <c r="D11" s="8">
+        <v>150</v>
+      </c>
+      <c r="E11" s="8">
+        <v>200</v>
+      </c>
+      <c r="F11" s="8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="7">
+        <v>150</v>
+      </c>
+      <c r="D12" s="7">
+        <v>130</v>
+      </c>
+      <c r="E12" s="7">
+        <v>100</v>
+      </c>
+      <c r="F12" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="8">
+        <v>200</v>
+      </c>
+      <c r="D13" s="8">
+        <v>200</v>
+      </c>
+      <c r="E13" s="8">
+        <v>140</v>
+      </c>
+      <c r="F13" s="8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" s="7">
+        <v>230</v>
+      </c>
+      <c r="D14" s="7">
+        <v>190</v>
+      </c>
+      <c r="E14" s="7">
+        <v>200</v>
+      </c>
+      <c r="F14" s="7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="8">
+        <v>230</v>
+      </c>
+      <c r="D15" s="8">
+        <v>210</v>
+      </c>
+      <c r="E15" s="8">
+        <v>210</v>
+      </c>
+      <c r="F15" s="8">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="7">
+        <v>210</v>
+      </c>
+      <c r="D16" s="7">
+        <v>150</v>
+      </c>
+      <c r="E16" s="7">
+        <v>75</v>
+      </c>
+      <c r="F16" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="8">
+        <v>220</v>
+      </c>
+      <c r="D17" s="8">
+        <v>85</v>
+      </c>
+      <c r="E17" s="8">
+        <v>150</v>
+      </c>
+      <c r="F17" s="8">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F21475A-AF0A-4856-8C67-9988EF456183}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>61</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A058435-DD2B-4E29-A9BF-E7ED958C3F29}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD7C5BD-6196-4E1D-B8CB-338E88055AEE}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FEAE5A-8A7F-4A1C-83C4-F6C4E1EB72B8}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9571,7 +10297,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10228,4 +10954,127 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6344FF5F-9C9F-47E9-A789-960072C7106D}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>55</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>105</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1112F405-3DC9-464A-9BFD-9981EF3D42BF}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>99</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>170</v>
+      </c>
+      <c r="E3">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>